<commit_message>
Fixed a bug where student entry dates match the first day of school. Also handle the situation where a student entered and exited in the same period.
Update Reconciliation student template to 22-23 school year.
</commit_message>
<xml_diff>
--- a/SchoolDistrictBilling/wwwroot/reportTemplates/ReconIndividualStudent.xlsx
+++ b/SchoolDistrictBilling/wwwroot/reportTemplates/ReconIndividualStudent.xlsx
@@ -113,9 +113,6 @@
     <t>Prior</t>
   </si>
   <si>
-    <t>RECONCILIATION REPORT FOR THE 2021-2022 SCHOOL YEAR</t>
-  </si>
-  <si>
     <t>Aggregate</t>
   </si>
   <si>
@@ -126,6 +123,9 @@
   </si>
   <si>
     <t xml:space="preserve">Remit To: </t>
+  </si>
+  <si>
+    <t>RECONCILIATION REPORT FOR THE 2022-2023 SCHOOL YEAR</t>
   </si>
 </sst>
 </file>
@@ -979,7 +979,7 @@
   <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="102" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1009,7 +1009,7 @@
       <c r="H1" s="50"/>
       <c r="I1" s="50"/>
       <c r="J1" s="85" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K1" s="82"/>
       <c r="L1" s="3"/>
@@ -1021,7 +1021,7 @@
       <c r="D2" s="5"/>
       <c r="E2" s="51"/>
       <c r="F2" s="6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="51"/>
@@ -1123,7 +1123,7 @@
         <v>6</v>
       </c>
       <c r="J8" s="76" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K8" s="39"/>
       <c r="L8" s="39" t="s">
@@ -1149,7 +1149,7 @@
         <v>11</v>
       </c>
       <c r="J9" s="77" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K9" s="44" t="s">
         <v>12</v>
@@ -1183,7 +1183,7 @@
         <v>19</v>
       </c>
       <c r="J10" s="78" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K10" s="44" t="s">
         <v>20</v>

</xml_diff>